<commit_message>
Add script to run on Prod env
</commit_message>
<xml_diff>
--- a/tests/Deals&Banking_data.xlsx
+++ b/tests/Deals&Banking_data.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19635" windowHeight="7500"/>
+    <workbookView windowWidth="27945" windowHeight="12180"/>
   </bookViews>
   <sheets>
     <sheet name="Deals_data" sheetId="1" r:id="rId1"/>
     <sheet name="Banking_Details" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
   <si>
     <t>providerType</t>
   </si>
@@ -48,18 +49,54 @@
     <t>VAS</t>
   </si>
   <si>
+    <t>Peeq</t>
+  </si>
+  <si>
+    <t>Peeq @ R95</t>
+  </si>
+  <si>
+    <t>0678678768</t>
+  </si>
+  <si>
+    <t>Durban</t>
+  </si>
+  <si>
+    <t>AccountHolderName</t>
+  </si>
+  <si>
+    <t>BankName</t>
+  </si>
+  <si>
+    <t>BranchName</t>
+  </si>
+  <si>
+    <t>DebitDay</t>
+  </si>
+  <si>
+    <t>AccountNumber</t>
+  </si>
+  <si>
+    <t>AccountType</t>
+  </si>
+  <si>
+    <t>Rohit Automate</t>
+  </si>
+  <si>
+    <t>BIDVEST BANK</t>
+  </si>
+  <si>
+    <t>BIDVEST BANK (GENERIC)</t>
+  </si>
+  <si>
+    <t>Savings</t>
+  </si>
+  <si>
     <t>FMTLocal</t>
   </si>
   <si>
     <t>FmtLocalEssentialsDeal_Safebase1_Bundle_DealDescription</t>
   </si>
   <si>
-    <t>0678678768</t>
-  </si>
-  <si>
-    <t>Durban</t>
-  </si>
-  <si>
     <t>Driven</t>
   </si>
   <si>
@@ -79,36 +116,6 @@
   </si>
   <si>
     <t>0678678770</t>
-  </si>
-  <si>
-    <t>AccountHolderName</t>
-  </si>
-  <si>
-    <t>BankName</t>
-  </si>
-  <si>
-    <t>BranchName</t>
-  </si>
-  <si>
-    <t>DebitDay</t>
-  </si>
-  <si>
-    <t>AccountNumber</t>
-  </si>
-  <si>
-    <t>AccountType</t>
-  </si>
-  <si>
-    <t>Rohit Automate</t>
-  </si>
-  <si>
-    <t>BIDVEST BANK</t>
-  </si>
-  <si>
-    <t>BIDVEST BANK (GENERIC)</t>
-  </si>
-  <si>
-    <t>Savings</t>
   </si>
 </sst>
 </file>
@@ -1264,10 +1271,133 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="1" width="13.8571428571429" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="60.1428571428571" customWidth="1"/>
+    <col min="4" max="4" width="13.1428571428571" customWidth="1"/>
+    <col min="5" max="5" width="13.7142857142857" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F$1:F$1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="5"/>
+  <cols>
+    <col min="1" max="1" width="21.2857142857143" customWidth="1"/>
+    <col min="2" max="2" width="14.8571428571429" customWidth="1"/>
+    <col min="3" max="3" width="25.4285714285714" customWidth="1"/>
+    <col min="4" max="4" width="9.71428571428571" customWidth="1"/>
+    <col min="5" max="5" width="16.7142857142857" customWidth="1"/>
+    <col min="6" max="6" width="13.4285714285714" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <v>687468346</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="4"/>
@@ -1301,10 +1431,10 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
@@ -1318,13 +1448,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
@@ -1332,84 +1462,19 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="5"/>
-  <cols>
-    <col min="1" max="1" width="21.2857142857143" customWidth="1"/>
-    <col min="2" max="2" width="14.8571428571429" customWidth="1"/>
-    <col min="3" max="3" width="25.4285714285714" customWidth="1"/>
-    <col min="4" max="4" width="9.71428571428571" customWidth="1"/>
-    <col min="5" max="5" width="16.7142857142857" customWidth="1"/>
-    <col min="6" max="6" width="13.4285714285714" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2">
-        <v>15</v>
-      </c>
-      <c r="E2">
-        <v>687468346</v>
-      </c>
-      <c r="F2" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add script to run on UAT env
</commit_message>
<xml_diff>
--- a/tests/Deals&Banking_data.xlsx
+++ b/tests/Deals&Banking_data.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="27">
   <si>
     <t>providerType</t>
   </si>
@@ -49,10 +49,10 @@
     <t>VAS</t>
   </si>
   <si>
-    <t>Peeq</t>
-  </si>
-  <si>
-    <t>Peeq @ R95</t>
+    <t>FMTLocal</t>
+  </si>
+  <si>
+    <t>FmtLocalEssentialsDeal_Safebase1_Bundle_DealDescription</t>
   </si>
   <si>
     <t>0678678768</t>
@@ -61,6 +61,27 @@
     <t>Durban</t>
   </si>
   <si>
+    <t>Driven</t>
+  </si>
+  <si>
+    <t>Driven @ R139</t>
+  </si>
+  <si>
+    <t>0678678769</t>
+  </si>
+  <si>
+    <t>Telco</t>
+  </si>
+  <si>
+    <t>On Air</t>
+  </si>
+  <si>
+    <t>On Air Testing Deal</t>
+  </si>
+  <si>
+    <t>0678678770</t>
+  </si>
+  <si>
     <t>AccountHolderName</t>
   </si>
   <si>
@@ -89,33 +110,6 @@
   </si>
   <si>
     <t>Savings</t>
-  </si>
-  <si>
-    <t>FMTLocal</t>
-  </si>
-  <si>
-    <t>FmtLocalEssentialsDeal_Safebase1_Bundle_DealDescription</t>
-  </si>
-  <si>
-    <t>Driven</t>
-  </si>
-  <si>
-    <t>Driven @ R139</t>
-  </si>
-  <si>
-    <t>0678678769</t>
-  </si>
-  <si>
-    <t>Telco</t>
-  </si>
-  <si>
-    <t>On Air</t>
-  </si>
-  <si>
-    <t>On Air Testing Deal</t>
-  </si>
-  <si>
-    <t>0678678770</t>
   </si>
 </sst>
 </file>
@@ -1271,13 +1265,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2:E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="13.8571428571429" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
@@ -1317,6 +1311,40 @@
         <v>8</v>
       </c>
       <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1347,33 +1375,33 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="F1" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D2">
         <v>15</v>
@@ -1382,7 +1410,7 @@
         <v>687468346</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1397,7 +1425,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="A2" sqref="A2:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="4"/>
@@ -1431,10 +1459,10 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
@@ -1448,13 +1476,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
@@ -1462,16 +1490,16 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Added code for searching the order and cancel the orders according to the order statues on Silver Surfer.
</commit_message>
<xml_diff>
--- a/tests/Deals&Banking_data.xlsx
+++ b/tests/Deals&Banking_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="12180"/>
+    <workbookView windowWidth="19635" windowHeight="7500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Deals_data" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="32">
   <si>
     <t>providerType</t>
   </si>
@@ -46,6 +46,21 @@
     <t>customerCity</t>
   </si>
   <si>
+    <t>Telco</t>
+  </si>
+  <si>
+    <t>On Air</t>
+  </si>
+  <si>
+    <t>On Air Testing Deal</t>
+  </si>
+  <si>
+    <t>0678678770</t>
+  </si>
+  <si>
+    <t>Durban</t>
+  </si>
+  <si>
     <t>VAS</t>
   </si>
   <si>
@@ -58,9 +73,6 @@
     <t>0678678768</t>
   </si>
   <si>
-    <t>Durban</t>
-  </si>
-  <si>
     <t>Driven</t>
   </si>
   <si>
@@ -70,18 +82,6 @@
     <t>0678678769</t>
   </si>
   <si>
-    <t>Telco</t>
-  </si>
-  <si>
-    <t>On Air</t>
-  </si>
-  <si>
-    <t>On Air Testing Deal</t>
-  </si>
-  <si>
-    <t>0678678770</t>
-  </si>
-  <si>
     <t>AccountHolderName</t>
   </si>
   <si>
@@ -94,9 +94,6 @@
     <t>DebitDay</t>
   </si>
   <si>
-    <t>AccountNumber</t>
-  </si>
-  <si>
     <t>AccountType</t>
   </si>
   <si>
@@ -110,6 +107,24 @@
   </si>
   <si>
     <t>Savings</t>
+  </si>
+  <si>
+    <t>UAT Deals</t>
+  </si>
+  <si>
+    <t>Production Deals</t>
+  </si>
+  <si>
+    <t>FMT Local Test Deal</t>
+  </si>
+  <si>
+    <t>Test Bundle 3 Provider</t>
+  </si>
+  <si>
+    <t>0678678771</t>
+  </si>
+  <si>
+    <t>Cape Town</t>
   </si>
 </sst>
 </file>
@@ -122,13 +137,19 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Courier New"/>
+      <charset val="134"/>
     </font>
     <font>
       <u/>
@@ -595,138 +616,141 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
@@ -1267,11 +1291,161 @@
   <sheetPr/>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="1" width="13.8571428571429" customWidth="1"/>
+    <col min="2" max="2" width="27.4285714285714" customWidth="1"/>
+    <col min="3" max="3" width="60.1428571428571" customWidth="1"/>
+    <col min="4" max="4" width="13.1428571428571" customWidth="1"/>
+    <col min="5" max="5" width="13.7142857142857" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="1" width="21.2857142857143" customWidth="1"/>
+    <col min="2" max="2" width="14.8571428571429" customWidth="1"/>
+    <col min="3" max="3" width="25.4285714285714" customWidth="1"/>
+    <col min="4" max="4" width="9.71428571428571" customWidth="1"/>
+    <col min="5" max="5" width="13.4285714285714" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="13.8571428571429" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
@@ -1297,21 +1471,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1319,13 +1481,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
@@ -1333,176 +1495,92 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F$1:F$1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="5"/>
-  <cols>
-    <col min="1" max="1" width="21.2857142857143" customWidth="1"/>
-    <col min="2" max="2" width="14.8571428571429" customWidth="1"/>
-    <col min="3" max="3" width="25.4285714285714" customWidth="1"/>
-    <col min="4" max="4" width="9.71428571428571" customWidth="1"/>
-    <col min="5" max="5" width="16.7142857142857" customWidth="1"/>
-    <col min="6" max="6" width="13.4285714285714" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" t="s">
-        <v>22</v>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2">
-        <v>15</v>
-      </c>
-      <c r="E2">
-        <v>687468346</v>
-      </c>
-      <c r="F2" t="s">
-        <v>26</v>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>27</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:E4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="4"/>
-  <cols>
-    <col min="1" max="1" width="13.8571428571429" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="60.1428571428571" customWidth="1"/>
-    <col min="4" max="4" width="13.1428571428571" customWidth="1"/>
-    <col min="5" max="5" width="13.7142857142857" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="B10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
+      <c r="D10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a custom report feature. Did code refactoring. Add more validations. Add a logic to stop execution after any of test got failed. Add a code to take SS and embadded into the test report.
</commit_message>
<xml_diff>
--- a/tests/Deals&Banking_data.xlsx
+++ b/tests/Deals&Banking_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19635" windowHeight="7500" activeTab="2"/>
+    <workbookView windowWidth="19635" windowHeight="7500"/>
   </bookViews>
   <sheets>
     <sheet name="Deals_data" sheetId="1" r:id="rId1"/>
@@ -67,10 +67,52 @@
     <t>FMTLocal</t>
   </si>
   <si>
+    <t>FMT Local Test Deal</t>
+  </si>
+  <si>
+    <t>0678678768</t>
+  </si>
+  <si>
+    <t>Test Bundle 3 Provider</t>
+  </si>
+  <si>
     <t>FmtLocalEssentialsDeal_Safebase1_Bundle_DealDescription</t>
   </si>
   <si>
-    <t>0678678768</t>
+    <t>0678678771</t>
+  </si>
+  <si>
+    <t>Cape Town</t>
+  </si>
+  <si>
+    <t>AccountHolderName</t>
+  </si>
+  <si>
+    <t>BankName</t>
+  </si>
+  <si>
+    <t>BranchName</t>
+  </si>
+  <si>
+    <t>DebitDay</t>
+  </si>
+  <si>
+    <t>AccountType</t>
+  </si>
+  <si>
+    <t>Rohit Automate</t>
+  </si>
+  <si>
+    <t>BIDVEST BANK</t>
+  </si>
+  <si>
+    <t>BIDVEST BANK (GENERIC)</t>
+  </si>
+  <si>
+    <t>Savings</t>
+  </si>
+  <si>
+    <t>UAT Deals</t>
   </si>
   <si>
     <t>Driven</t>
@@ -82,49 +124,7 @@
     <t>0678678769</t>
   </si>
   <si>
-    <t>AccountHolderName</t>
-  </si>
-  <si>
-    <t>BankName</t>
-  </si>
-  <si>
-    <t>BranchName</t>
-  </si>
-  <si>
-    <t>DebitDay</t>
-  </si>
-  <si>
-    <t>AccountType</t>
-  </si>
-  <si>
-    <t>Rohit Automate</t>
-  </si>
-  <si>
-    <t>BIDVEST BANK</t>
-  </si>
-  <si>
-    <t>BIDVEST BANK (GENERIC)</t>
-  </si>
-  <si>
-    <t>Savings</t>
-  </si>
-  <si>
-    <t>UAT Deals</t>
-  </si>
-  <si>
     <t>Production Deals</t>
-  </si>
-  <si>
-    <t>FMT Local Test Deal</t>
-  </si>
-  <si>
-    <t>Test Bundle 3 Provider</t>
-  </si>
-  <si>
-    <t>0678678771</t>
-  </si>
-  <si>
-    <t>Cape Town</t>
   </si>
 </sst>
 </file>
@@ -1291,8 +1291,8 @@
   <sheetPr/>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="4"/>
@@ -1325,10 +1325,10 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -1342,10 +1342,10 @@
       <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -1359,17 +1359,17 @@
       <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1384,7 +1384,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="4"/>
@@ -1398,36 +1398,36 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D2">
         <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1441,8 +1441,8 @@
   <sheetPr/>
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -1473,7 +1473,7 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1501,7 +1501,7 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>13</v>
@@ -1515,13 +1515,13 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>
@@ -1529,7 +1529,7 @@
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1557,7 +1557,7 @@
         <v>11</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>13</v>
@@ -1571,16 +1571,16 @@
         <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="E10" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made changes according to pipeline
</commit_message>
<xml_diff>
--- a/tests/Deals&Banking_data.xlsx
+++ b/tests/Deals&Banking_data.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="32">
   <si>
     <t>providerType</t>
   </si>
@@ -64,67 +64,67 @@
     <t>VAS</t>
   </si>
   <si>
+    <t>Driven</t>
+  </si>
+  <si>
+    <t>Driven @ R139</t>
+  </si>
+  <si>
+    <t>0678678769</t>
+  </si>
+  <si>
+    <t>AccountHolderName</t>
+  </si>
+  <si>
+    <t>BankName</t>
+  </si>
+  <si>
+    <t>BranchName</t>
+  </si>
+  <si>
+    <t>DebitDay</t>
+  </si>
+  <si>
+    <t>AccountType</t>
+  </si>
+  <si>
+    <t>Rohit Automate</t>
+  </si>
+  <si>
+    <t>BIDVEST BANK</t>
+  </si>
+  <si>
+    <t>BIDVEST BANK (GENERIC)</t>
+  </si>
+  <si>
+    <t>Savings</t>
+  </si>
+  <si>
+    <t>UAT Deals</t>
+  </si>
+  <si>
     <t>FMTLocal</t>
   </si>
   <si>
+    <t>FmtLocalEssentialsDeal_Safebase1_Bundle_DealDescription</t>
+  </si>
+  <si>
+    <t>0678678768</t>
+  </si>
+  <si>
+    <t>Production Deals</t>
+  </si>
+  <si>
     <t>FMT Local Test Deal</t>
   </si>
   <si>
-    <t>0678678768</t>
-  </si>
-  <si>
     <t>Test Bundle 3 Provider</t>
   </si>
   <si>
-    <t>FmtLocalEssentialsDeal_Safebase1_Bundle_DealDescription</t>
-  </si>
-  <si>
     <t>0678678771</t>
   </si>
   <si>
     <t>Cape Town</t>
-  </si>
-  <si>
-    <t>AccountHolderName</t>
-  </si>
-  <si>
-    <t>BankName</t>
-  </si>
-  <si>
-    <t>BranchName</t>
-  </si>
-  <si>
-    <t>DebitDay</t>
-  </si>
-  <si>
-    <t>AccountType</t>
-  </si>
-  <si>
-    <t>Rohit Automate</t>
-  </si>
-  <si>
-    <t>BIDVEST BANK</t>
-  </si>
-  <si>
-    <t>BIDVEST BANK (GENERIC)</t>
-  </si>
-  <si>
-    <t>Savings</t>
-  </si>
-  <si>
-    <t>UAT Deals</t>
-  </si>
-  <si>
-    <t>Driven</t>
-  </si>
-  <si>
-    <t>Driven @ R139</t>
-  </si>
-  <si>
-    <t>0678678769</t>
-  </si>
-  <si>
-    <t>Production Deals</t>
   </si>
 </sst>
 </file>
@@ -1289,13 +1289,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="13.8571428571429" customWidth="1"/>
     <col min="2" max="2" width="27.4285714285714" customWidth="1"/>
@@ -1325,10 +1325,10 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -1342,10 +1342,10 @@
       <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -1353,23 +1353,6 @@
       </c>
       <c r="E3" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1398,36 +1381,36 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
         <v>18</v>
-      </c>
-      <c r="B1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D2">
         <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1442,7 +1425,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:E10"/>
+      <selection activeCell="A3" sqref="A3:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -1473,7 +1456,7 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1498,13 +1481,13 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
@@ -1515,13 +1498,13 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>
@@ -1529,7 +1512,7 @@
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1554,13 +1537,13 @@
         <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="E9" t="s">
         <v>9</v>
@@ -1571,16 +1554,16 @@
         <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="E10" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
deals changes in file to production deals
</commit_message>
<xml_diff>
--- a/tests/Deals&Banking_data.xlsx
+++ b/tests/Deals&Banking_data.xlsx
@@ -64,6 +64,48 @@
     <t>VAS</t>
   </si>
   <si>
+    <t>FMTLocal</t>
+  </si>
+  <si>
+    <t>FMT Local Test Deal</t>
+  </si>
+  <si>
+    <t>0678678768</t>
+  </si>
+  <si>
+    <t>AccountHolderName</t>
+  </si>
+  <si>
+    <t>BankName</t>
+  </si>
+  <si>
+    <t>BranchName</t>
+  </si>
+  <si>
+    <t>DebitDay</t>
+  </si>
+  <si>
+    <t>AccountType</t>
+  </si>
+  <si>
+    <t>Rohit Automate</t>
+  </si>
+  <si>
+    <t>BIDVEST BANK</t>
+  </si>
+  <si>
+    <t>BIDVEST BANK (GENERIC)</t>
+  </si>
+  <si>
+    <t>Savings</t>
+  </si>
+  <si>
+    <t>UAT Deals</t>
+  </si>
+  <si>
+    <t>FmtLocalEssentialsDeal_Safebase1_Bundle_DealDescription</t>
+  </si>
+  <si>
     <t>Driven</t>
   </si>
   <si>
@@ -73,49 +115,7 @@
     <t>0678678769</t>
   </si>
   <si>
-    <t>AccountHolderName</t>
-  </si>
-  <si>
-    <t>BankName</t>
-  </si>
-  <si>
-    <t>BranchName</t>
-  </si>
-  <si>
-    <t>DebitDay</t>
-  </si>
-  <si>
-    <t>AccountType</t>
-  </si>
-  <si>
-    <t>Rohit Automate</t>
-  </si>
-  <si>
-    <t>BIDVEST BANK</t>
-  </si>
-  <si>
-    <t>BIDVEST BANK (GENERIC)</t>
-  </si>
-  <si>
-    <t>Savings</t>
-  </si>
-  <si>
-    <t>UAT Deals</t>
-  </si>
-  <si>
-    <t>FMTLocal</t>
-  </si>
-  <si>
-    <t>FmtLocalEssentialsDeal_Safebase1_Bundle_DealDescription</t>
-  </si>
-  <si>
-    <t>0678678768</t>
-  </si>
-  <si>
     <t>Production Deals</t>
-  </si>
-  <si>
-    <t>FMT Local Test Deal</t>
   </si>
   <si>
     <t>Test Bundle 3 Provider</t>
@@ -1292,7 +1292,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A2" sqref="A2:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="4"/>
@@ -1325,10 +1325,10 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -1342,10 +1342,10 @@
       <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -1425,7 +1425,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:E5"/>
+      <selection activeCell="A8" sqref="A8:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -1481,13 +1481,13 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
         <v>24</v>
       </c>
-      <c r="C4" t="s">
-        <v>25</v>
-      </c>
       <c r="D4" s="2" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
@@ -1498,13 +1498,13 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>
@@ -1512,7 +1512,7 @@
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1537,13 +1537,13 @@
         <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="E9" t="s">
         <v>9</v>
@@ -1557,7 +1557,7 @@
         <v>29</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>30</v>

</xml_diff>